<commit_message>
🎞 Al Filo del Mañana
</commit_message>
<xml_diff>
--- a/CARTELERA.xlsx
+++ b/CARTELERA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54113\Desktop\CARTELERA 1000 PELICULAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1D1508-73D4-462C-9B40-87612AAAE57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EF53D8-432C-4FD4-9B15-CFA0431BE853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="1016">
   <si>
     <t>PELÍCULA</t>
   </si>
@@ -2944,9 +2944,6 @@
     <t>GOSFORD PARK</t>
   </si>
   <si>
-    <t>MENACE II SPCIETY</t>
-  </si>
-  <si>
     <t>PRECIOUS</t>
   </si>
   <si>
@@ -3113,6 +3110,9 @@
   </si>
   <si>
     <t>PINOCHO</t>
+  </si>
+  <si>
+    <t>MENACE II SOCIETY</t>
   </si>
 </sst>
 </file>
@@ -3925,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A564" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E578" sqref="E578"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3945,19 +3945,19 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F1" s="22"/>
     </row>
@@ -3972,16 +3972,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="8"/>
       <c r="H2" s="42">
         <f>COUNTIF($E$2:$E$1001,"VISTO")</f>
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4013,7 +4013,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E4" s="34"/>
       <c r="G4" s="11"/>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="H5" s="13">
         <f>SUM(H2:H4)</f>
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="23" t="s">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="H6" s="14">
         <f>1000-H5</f>
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4092,7 +4092,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F8" s="24"/>
     </row>
@@ -4108,12 +4108,12 @@
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="48" t="str">
         <f ca="1">INDEX(B2:B1001,RANDBETWEEN(1,COUNTA(B2:B1001)),1)</f>
-        <v>UN LARGO ADIÓS</v>
+        <v>TRAFFIC</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
@@ -4172,7 +4172,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F13" s="24"/>
     </row>
@@ -4267,10 +4267,10 @@
         <v>3</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F20" s="24"/>
     </row>
@@ -4288,7 +4288,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4302,10 +4302,10 @@
         <v>3</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F22" s="24"/>
     </row>
@@ -4320,10 +4320,10 @@
         <v>3</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F23" s="24"/>
     </row>
@@ -4353,10 +4353,10 @@
         <v>3</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F25" s="24"/>
     </row>
@@ -4371,10 +4371,10 @@
         <v>3</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F26" s="24"/>
     </row>
@@ -4402,10 +4402,10 @@
         <v>4</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4420,7 +4420,7 @@
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F29" s="24"/>
     </row>
@@ -4448,7 +4448,7 @@
         <v>4</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E31" s="34"/>
     </row>
@@ -4463,10 +4463,10 @@
         <v>4</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F32" s="24"/>
     </row>
@@ -4481,7 +4481,7 @@
         <v>4</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E33" s="34"/>
     </row>
@@ -4522,10 +4522,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F36" s="24"/>
     </row>
@@ -4553,7 +4553,7 @@
         <v>5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E38" s="34"/>
     </row>
@@ -4568,10 +4568,10 @@
         <v>5</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E39" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F39" s="24"/>
     </row>
@@ -4601,7 +4601,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E41" s="34"/>
     </row>
@@ -4623,7 +4623,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="33" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C43" s="5">
         <v>6</v>
@@ -4642,7 +4642,7 @@
         <v>6</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E44" s="34"/>
     </row>
@@ -4696,7 +4696,7 @@
         <v>6</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E48" s="34"/>
     </row>
@@ -4711,7 +4711,7 @@
         <v>6</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E49" s="34"/>
     </row>
@@ -4726,7 +4726,7 @@
         <v>6</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E50" s="34"/>
     </row>
@@ -4754,7 +4754,7 @@
         <v>7</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E52" s="34"/>
     </row>
@@ -4795,10 +4795,10 @@
         <v>7</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F55" s="24"/>
     </row>
@@ -4807,7 +4807,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C56" s="2">
         <v>7</v>
@@ -4826,7 +4826,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E57" s="34"/>
     </row>
@@ -4854,7 +4854,7 @@
         <v>8</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E59" s="34"/>
     </row>
@@ -4882,7 +4882,7 @@
         <v>8</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E61" s="34"/>
     </row>
@@ -4949,10 +4949,10 @@
         <v>9</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E66" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F66" s="24"/>
     </row>
@@ -5006,10 +5006,10 @@
         <v>9</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E70" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F70" s="24"/>
     </row>
@@ -5037,7 +5037,7 @@
         <v>9</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E72" s="34"/>
     </row>
@@ -5052,7 +5052,7 @@
         <v>10</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E73" s="34"/>
     </row>
@@ -5067,10 +5067,10 @@
         <v>10</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E74" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5111,7 +5111,7 @@
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F77" s="24"/>
     </row>
@@ -5139,7 +5139,7 @@
         <v>10</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E79" s="34"/>
     </row>
@@ -5167,10 +5167,10 @@
         <v>11</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E81" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F81" s="24"/>
     </row>
@@ -5188,7 +5188,7 @@
         <v>16</v>
       </c>
       <c r="E82" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5202,10 +5202,10 @@
         <v>11</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E83" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F83" s="24"/>
     </row>
@@ -5220,7 +5220,7 @@
         <v>11</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E84" s="34"/>
     </row>
@@ -5235,7 +5235,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="E85" s="34"/>
     </row>
@@ -5345,10 +5345,10 @@
         <v>12</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E93" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F93" s="24"/>
     </row>
@@ -5366,7 +5366,7 @@
         <v>16</v>
       </c>
       <c r="E94" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F94" s="24"/>
     </row>
@@ -5474,7 +5474,7 @@
         <v>13</v>
       </c>
       <c r="D102" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E102" s="34"/>
     </row>
@@ -5504,10 +5504,10 @@
         <v>13</v>
       </c>
       <c r="D104" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E104" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F104" s="24"/>
     </row>
@@ -5522,10 +5522,10 @@
         <v>13</v>
       </c>
       <c r="D105" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E105" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F105" s="24"/>
     </row>
@@ -5553,10 +5553,10 @@
         <v>14</v>
       </c>
       <c r="D107" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E107" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5583,7 +5583,7 @@
         <v>14</v>
       </c>
       <c r="D109" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E109" s="34"/>
     </row>
@@ -5629,7 +5629,7 @@
         <v>16</v>
       </c>
       <c r="E112" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F112" s="24"/>
     </row>
@@ -5647,7 +5647,7 @@
         <v>16</v>
       </c>
       <c r="E113" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -5778,7 +5778,7 @@
         <v>15</v>
       </c>
       <c r="D123" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E123" s="34"/>
     </row>
@@ -5871,10 +5871,10 @@
         <v>16</v>
       </c>
       <c r="D130" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E130" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F130" s="24"/>
     </row>
@@ -5902,7 +5902,7 @@
         <v>16</v>
       </c>
       <c r="D132" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E132" s="34"/>
     </row>
@@ -5958,10 +5958,10 @@
         <v>16</v>
       </c>
       <c r="D136" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E136" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F136" s="24"/>
     </row>
@@ -5991,7 +5991,7 @@
         <v>17</v>
       </c>
       <c r="D138" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E138" s="34"/>
     </row>
@@ -6021,7 +6021,7 @@
         <v>17</v>
       </c>
       <c r="D140" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E140" s="34"/>
     </row>
@@ -6036,7 +6036,7 @@
         <v>17</v>
       </c>
       <c r="D141" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E141" s="34"/>
     </row>
@@ -6064,7 +6064,7 @@
         <v>17</v>
       </c>
       <c r="D143" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E143" s="34"/>
     </row>
@@ -6079,7 +6079,7 @@
         <v>17</v>
       </c>
       <c r="D144" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E144" s="34"/>
     </row>
@@ -6094,7 +6094,7 @@
         <v>18</v>
       </c>
       <c r="D145" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E145" s="34"/>
     </row>
@@ -6109,7 +6109,7 @@
         <v>18</v>
       </c>
       <c r="D146" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E146" s="34"/>
     </row>
@@ -6137,7 +6137,7 @@
         <v>18</v>
       </c>
       <c r="D148" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E148" s="34"/>
     </row>
@@ -6191,10 +6191,10 @@
         <v>18</v>
       </c>
       <c r="D152" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E152" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F152" s="24"/>
     </row>
@@ -6209,10 +6209,10 @@
         <v>19</v>
       </c>
       <c r="D153" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E153" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F153" s="24"/>
     </row>
@@ -6221,7 +6221,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="33" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C154" s="2">
         <v>19</v>
@@ -6266,7 +6266,7 @@
         <v>19</v>
       </c>
       <c r="D157" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E157" s="34"/>
     </row>
@@ -6284,7 +6284,7 @@
         <v>16</v>
       </c>
       <c r="E158" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F158" s="24"/>
     </row>
@@ -6353,7 +6353,7 @@
         <v>20</v>
       </c>
       <c r="D163" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E163" s="34"/>
     </row>
@@ -6368,7 +6368,7 @@
         <v>20</v>
       </c>
       <c r="D164" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E164" s="34"/>
     </row>
@@ -6383,7 +6383,7 @@
         <v>20</v>
       </c>
       <c r="D165" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E165" s="34"/>
     </row>
@@ -6401,7 +6401,7 @@
         <v>16</v>
       </c>
       <c r="E166" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F166" s="24"/>
     </row>
@@ -6416,7 +6416,7 @@
         <v>20</v>
       </c>
       <c r="D167" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E167" s="34"/>
     </row>
@@ -6434,7 +6434,7 @@
         <v>27</v>
       </c>
       <c r="E168" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F168" s="24"/>
     </row>
@@ -6449,7 +6449,7 @@
         <v>20</v>
       </c>
       <c r="D169" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E169" s="34"/>
     </row>
@@ -6471,7 +6471,7 @@
         <v>170</v>
       </c>
       <c r="B171" s="33" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C171" s="2">
         <v>21</v>
@@ -6503,7 +6503,7 @@
         <v>21</v>
       </c>
       <c r="D173" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E173" s="34"/>
     </row>
@@ -6570,7 +6570,7 @@
         <v>22</v>
       </c>
       <c r="D178" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E178" s="34"/>
     </row>
@@ -6585,7 +6585,7 @@
         <v>22</v>
       </c>
       <c r="D179" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E179" s="34"/>
     </row>
@@ -6641,7 +6641,7 @@
         <v>22</v>
       </c>
       <c r="D183" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E183" s="34"/>
     </row>
@@ -6682,10 +6682,10 @@
         <v>23</v>
       </c>
       <c r="D186" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E186" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -6725,10 +6725,10 @@
         <v>23</v>
       </c>
       <c r="D189" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E189" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F189" s="24"/>
     </row>
@@ -6743,7 +6743,7 @@
         <v>23</v>
       </c>
       <c r="D190" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E190" s="34"/>
     </row>
@@ -6758,10 +6758,10 @@
         <v>23</v>
       </c>
       <c r="D191" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E191" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F191" s="24"/>
     </row>
@@ -6789,10 +6789,10 @@
         <v>23</v>
       </c>
       <c r="D193" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E193" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F193" s="24"/>
     </row>
@@ -6956,7 +6956,7 @@
         <v>25</v>
       </c>
       <c r="D205" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E205" s="34"/>
     </row>
@@ -6984,7 +6984,7 @@
         <v>25</v>
       </c>
       <c r="D207" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E207" s="34"/>
     </row>
@@ -7017,7 +7017,7 @@
         <v>16</v>
       </c>
       <c r="E209" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F209" s="24"/>
     </row>
@@ -7099,7 +7099,7 @@
         <v>26</v>
       </c>
       <c r="D215" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E215" s="34"/>
     </row>
@@ -7114,7 +7114,7 @@
         <v>26</v>
       </c>
       <c r="D216" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E216" s="34"/>
     </row>
@@ -7129,7 +7129,7 @@
         <v>26</v>
       </c>
       <c r="D217" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E217" s="34"/>
     </row>
@@ -7224,7 +7224,7 @@
         <v>27</v>
       </c>
       <c r="D224" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E224" s="34"/>
     </row>
@@ -7268,7 +7268,7 @@
         <v>16</v>
       </c>
       <c r="E227" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="228" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7362,10 +7362,10 @@
         <v>28</v>
       </c>
       <c r="D234" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E234" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F234" s="24"/>
     </row>
@@ -7439,7 +7439,7 @@
         <v>239</v>
       </c>
       <c r="B240" s="33" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C240" s="2">
         <v>29</v>
@@ -7474,7 +7474,7 @@
         <v>16</v>
       </c>
       <c r="E242" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F242" s="24"/>
     </row>
@@ -7544,7 +7544,7 @@
         <v>16</v>
       </c>
       <c r="E247" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="248" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7573,10 +7573,10 @@
         <v>30</v>
       </c>
       <c r="D249" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E249" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F249" s="24"/>
     </row>
@@ -7598,13 +7598,13 @@
         <v>250</v>
       </c>
       <c r="B251" s="36" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C251" s="2">
         <v>30</v>
       </c>
       <c r="D251" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E251" s="34"/>
     </row>
@@ -7732,13 +7732,13 @@
         <v>260</v>
       </c>
       <c r="B261" s="33" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C261" s="5">
         <v>32</v>
       </c>
       <c r="D261" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E261" s="34"/>
     </row>
@@ -7809,10 +7809,10 @@
         <v>32</v>
       </c>
       <c r="D266" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E266" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -7826,7 +7826,7 @@
         <v>32</v>
       </c>
       <c r="D267" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E267" s="34"/>
     </row>
@@ -7835,7 +7835,7 @@
         <v>267</v>
       </c>
       <c r="B268" s="33" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C268" s="5">
         <v>33</v>
@@ -7867,7 +7867,7 @@
         <v>33</v>
       </c>
       <c r="D270" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E270" s="34"/>
     </row>
@@ -7923,10 +7923,10 @@
         <v>33</v>
       </c>
       <c r="D274" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E274" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F274" s="24"/>
     </row>
@@ -7974,13 +7974,13 @@
         <v>277</v>
       </c>
       <c r="B278" s="33" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C278" s="2">
         <v>34</v>
       </c>
       <c r="D278" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E278" s="34"/>
     </row>
@@ -8034,10 +8034,10 @@
         <v>34</v>
       </c>
       <c r="D282" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E282" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F282" s="24"/>
     </row>
@@ -8055,7 +8055,7 @@
         <v>27</v>
       </c>
       <c r="E283" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F283" s="24"/>
     </row>
@@ -8073,7 +8073,7 @@
         <v>16</v>
       </c>
       <c r="E284" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F284" s="24"/>
     </row>
@@ -8088,10 +8088,10 @@
         <v>35</v>
       </c>
       <c r="D285" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E285" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F285" s="24"/>
     </row>
@@ -8106,10 +8106,10 @@
         <v>35</v>
       </c>
       <c r="D286" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E286" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F286" s="24"/>
     </row>
@@ -8166,7 +8166,7 @@
         <v>16</v>
       </c>
       <c r="E290" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F290" s="24"/>
     </row>
@@ -8209,7 +8209,7 @@
         <v>36</v>
       </c>
       <c r="D293" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E293" s="34"/>
     </row>
@@ -8277,7 +8277,7 @@
       </c>
       <c r="D298" s="17"/>
       <c r="E298" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="299" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -8291,7 +8291,7 @@
         <v>36</v>
       </c>
       <c r="D299" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E299" s="34"/>
     </row>
@@ -8332,7 +8332,7 @@
         <v>37</v>
       </c>
       <c r="D302" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E302" s="34"/>
     </row>
@@ -8360,10 +8360,10 @@
         <v>37</v>
       </c>
       <c r="D304" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E304" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F304" s="24"/>
     </row>
@@ -8393,10 +8393,10 @@
         <v>37</v>
       </c>
       <c r="D306" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E306" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F306" s="24"/>
     </row>
@@ -8411,7 +8411,7 @@
         <v>37</v>
       </c>
       <c r="D307" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E307" s="34"/>
     </row>
@@ -8467,10 +8467,10 @@
         <v>38</v>
       </c>
       <c r="D311" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E311" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F311" s="24"/>
     </row>
@@ -8488,7 +8488,7 @@
         <v>16</v>
       </c>
       <c r="E312" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F312" s="24"/>
     </row>
@@ -8529,7 +8529,7 @@
         <v>38</v>
       </c>
       <c r="D315" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E315" s="34"/>
     </row>
@@ -8559,7 +8559,7 @@
         <v>38</v>
       </c>
       <c r="D317" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E317" s="34"/>
     </row>
@@ -8604,10 +8604,10 @@
         <v>39</v>
       </c>
       <c r="D320" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E320" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F320" s="24"/>
     </row>
@@ -8625,7 +8625,7 @@
         <v>16</v>
       </c>
       <c r="E321" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F321" s="24"/>
     </row>
@@ -8669,7 +8669,7 @@
         <v>27</v>
       </c>
       <c r="E324" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F324" s="24"/>
     </row>
@@ -8684,7 +8684,7 @@
         <v>39</v>
       </c>
       <c r="D325" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E325" s="34"/>
     </row>
@@ -8699,7 +8699,7 @@
         <v>39</v>
       </c>
       <c r="D326" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E326" s="34"/>
     </row>
@@ -8824,10 +8824,10 @@
         <v>40</v>
       </c>
       <c r="D335" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E335" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F335" s="24"/>
     </row>
@@ -8868,7 +8868,7 @@
         <v>40</v>
       </c>
       <c r="D338" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E338" s="34"/>
     </row>
@@ -8883,7 +8883,7 @@
         <v>41</v>
       </c>
       <c r="D339" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E339" s="34"/>
     </row>
@@ -8898,10 +8898,10 @@
         <v>41</v>
       </c>
       <c r="D340" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E340" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F340" s="24"/>
     </row>
@@ -8942,7 +8942,7 @@
         <v>41</v>
       </c>
       <c r="D343" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E343" s="34"/>
     </row>
@@ -9076,7 +9076,7 @@
         <v>42</v>
       </c>
       <c r="D353" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E353" s="34"/>
     </row>
@@ -9158,10 +9158,10 @@
         <v>43</v>
       </c>
       <c r="D359" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E359" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F359" s="24"/>
     </row>
@@ -9202,7 +9202,7 @@
         <v>43</v>
       </c>
       <c r="D362" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E362" s="34"/>
     </row>
@@ -9217,7 +9217,7 @@
         <v>43</v>
       </c>
       <c r="D363" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E363" s="34"/>
     </row>
@@ -9247,10 +9247,10 @@
         <v>43</v>
       </c>
       <c r="D365" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E365" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F365" s="24"/>
     </row>
@@ -9274,7 +9274,7 @@
         <v>366</v>
       </c>
       <c r="B367" s="33" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C367" s="2">
         <v>44</v>
@@ -9293,7 +9293,7 @@
         <v>44</v>
       </c>
       <c r="D368" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E368" s="34"/>
     </row>
@@ -9362,7 +9362,7 @@
         <v>44</v>
       </c>
       <c r="D373" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E373" s="34"/>
     </row>
@@ -9420,7 +9420,7 @@
         <v>45</v>
       </c>
       <c r="D377" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E377" s="34"/>
     </row>
@@ -9518,7 +9518,7 @@
         <v>27</v>
       </c>
       <c r="E384" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F384" s="24"/>
     </row>
@@ -9559,7 +9559,7 @@
         <v>46</v>
       </c>
       <c r="D387" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E387" s="34"/>
     </row>
@@ -9600,7 +9600,7 @@
         <v>46</v>
       </c>
       <c r="D390" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E390" s="34"/>
     </row>
@@ -9615,7 +9615,7 @@
         <v>47</v>
       </c>
       <c r="D391" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E391" s="34"/>
     </row>
@@ -9630,7 +9630,7 @@
         <v>47</v>
       </c>
       <c r="D392" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E392" s="34"/>
     </row>
@@ -9645,7 +9645,7 @@
         <v>47</v>
       </c>
       <c r="D393" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E393" s="34"/>
     </row>
@@ -9673,7 +9673,7 @@
         <v>47</v>
       </c>
       <c r="D395" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E395" s="34"/>
     </row>
@@ -9701,7 +9701,7 @@
         <v>47</v>
       </c>
       <c r="D397" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E397" s="34"/>
     </row>
@@ -9794,10 +9794,10 @@
         <v>48</v>
       </c>
       <c r="D404" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E404" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F404" s="24"/>
     </row>
@@ -9812,10 +9812,10 @@
         <v>48</v>
       </c>
       <c r="D405" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E405" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F405" s="24"/>
     </row>
@@ -9856,7 +9856,7 @@
         <v>49</v>
       </c>
       <c r="D408" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E408" s="34"/>
     </row>
@@ -9871,10 +9871,10 @@
         <v>49</v>
       </c>
       <c r="D409" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E409" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F409" s="24"/>
     </row>
@@ -9892,7 +9892,7 @@
         <v>27</v>
       </c>
       <c r="E410" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F410" s="24"/>
     </row>
@@ -9960,7 +9960,7 @@
       </c>
       <c r="D415" s="17"/>
       <c r="E415" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="416" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -9987,10 +9987,10 @@
         <v>50</v>
       </c>
       <c r="D417" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E417" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F417" s="24"/>
     </row>
@@ -10243,10 +10243,10 @@
         <v>52</v>
       </c>
       <c r="D436" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E436" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F436" s="24"/>
     </row>
@@ -10274,10 +10274,10 @@
         <v>52</v>
       </c>
       <c r="D438" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E438" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="439" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -10528,7 +10528,7 @@
         <v>16</v>
       </c>
       <c r="E457" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F457" s="24"/>
     </row>
@@ -10608,10 +10608,10 @@
         <v>55</v>
       </c>
       <c r="D463" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E463" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F463" s="24"/>
     </row>
@@ -10652,10 +10652,10 @@
         <v>55</v>
       </c>
       <c r="D466" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E466" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="467" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -10685,7 +10685,7 @@
         <v>16</v>
       </c>
       <c r="E468" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="469" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -10764,10 +10764,10 @@
         <v>56</v>
       </c>
       <c r="D474" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E474" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F474" s="24"/>
     </row>
@@ -10951,10 +10951,10 @@
         <v>58</v>
       </c>
       <c r="D488" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E488" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F488" s="24"/>
     </row>
@@ -11022,7 +11022,7 @@
       </c>
       <c r="D493" s="17"/>
       <c r="E493" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F493" s="24"/>
     </row>
@@ -11122,7 +11122,7 @@
         <v>500</v>
       </c>
       <c r="B501" s="36" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C501" s="2">
         <v>59</v>
@@ -11235,7 +11235,7 @@
         <v>16</v>
       </c>
       <c r="E509" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F509" s="24"/>
     </row>
@@ -11263,7 +11263,7 @@
         <v>60</v>
       </c>
       <c r="D511" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E511" s="34"/>
     </row>
@@ -11318,7 +11318,7 @@
       </c>
       <c r="D515" s="17"/>
       <c r="E515" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F515" s="24"/>
     </row>
@@ -11333,7 +11333,7 @@
         <v>60</v>
       </c>
       <c r="D516" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E516" s="34"/>
     </row>
@@ -11362,7 +11362,7 @@
       </c>
       <c r="D518" s="17"/>
       <c r="E518" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F518" s="24"/>
     </row>
@@ -11521,7 +11521,7 @@
       </c>
       <c r="D530" s="17"/>
       <c r="E530" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="531" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -11535,10 +11535,10 @@
         <v>62</v>
       </c>
       <c r="D531" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E531" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="532" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -11581,7 +11581,7 @@
         <v>27</v>
       </c>
       <c r="E534" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="535" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -11611,7 +11611,7 @@
         <v>27</v>
       </c>
       <c r="E536" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F536" s="24"/>
     </row>
@@ -11743,10 +11743,10 @@
         <v>64</v>
       </c>
       <c r="D546" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E546" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F546" s="24"/>
     </row>
@@ -11852,10 +11852,10 @@
         <v>65</v>
       </c>
       <c r="D554" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E554" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F554" s="24"/>
     </row>
@@ -11883,10 +11883,10 @@
         <v>65</v>
       </c>
       <c r="D556" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E556" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F556" s="24"/>
     </row>
@@ -11930,7 +11930,7 @@
         <v>27</v>
       </c>
       <c r="E559" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="560" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12168,7 +12168,7 @@
         <v>16</v>
       </c>
       <c r="E577" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="578" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12261,7 +12261,7 @@
       </c>
       <c r="D584" s="17"/>
       <c r="E584" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F584" s="24"/>
     </row>
@@ -12276,7 +12276,7 @@
         <v>68</v>
       </c>
       <c r="D585" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E585" s="34"/>
     </row>
@@ -12320,7 +12320,7 @@
         <v>16</v>
       </c>
       <c r="E588" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F588" s="24"/>
     </row>
@@ -12377,7 +12377,7 @@
         <v>16</v>
       </c>
       <c r="E592" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F592" s="24"/>
     </row>
@@ -12473,7 +12473,7 @@
         <v>16</v>
       </c>
       <c r="E599" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="600" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12513,10 +12513,10 @@
         <v>70</v>
       </c>
       <c r="D602" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E602" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F602" s="24"/>
     </row>
@@ -12560,7 +12560,7 @@
         <v>16</v>
       </c>
       <c r="E605" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F605" s="24"/>
     </row>
@@ -12604,7 +12604,7 @@
         <v>16</v>
       </c>
       <c r="E608" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F608" s="24"/>
     </row>
@@ -12763,7 +12763,7 @@
       </c>
       <c r="D620" s="17"/>
       <c r="E620" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F620" s="24"/>
     </row>
@@ -12902,16 +12902,16 @@
         <v>630</v>
       </c>
       <c r="B631" s="4" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C631" s="2">
         <v>73</v>
       </c>
       <c r="D631" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E631" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F631" s="24"/>
     </row>
@@ -13033,7 +13033,7 @@
         <v>27</v>
       </c>
       <c r="E640" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F640" s="24"/>
     </row>
@@ -13126,7 +13126,7 @@
         <v>75</v>
       </c>
       <c r="D647" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E647" s="34"/>
     </row>
@@ -13186,14 +13186,18 @@
       <c r="A652" s="31">
         <v>651</v>
       </c>
-      <c r="B652" s="33" t="s">
+      <c r="B652" s="35" t="s">
         <v>643</v>
       </c>
       <c r="C652" s="2">
         <v>76</v>
       </c>
-      <c r="D652" s="17"/>
-      <c r="E652" s="34"/>
+      <c r="D652" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E652" s="34" t="s">
+        <v>1009</v>
+      </c>
     </row>
     <row r="653" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A653" s="31">
@@ -13219,7 +13223,7 @@
         <v>76</v>
       </c>
       <c r="D654" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E654" s="34"/>
     </row>
@@ -13458,7 +13462,7 @@
       </c>
       <c r="D672" s="17"/>
       <c r="E672" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F672" s="24"/>
     </row>
@@ -13642,10 +13646,10 @@
         <v>80</v>
       </c>
       <c r="D686" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E686" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F686" s="24"/>
     </row>
@@ -13686,10 +13690,10 @@
         <v>80</v>
       </c>
       <c r="D689" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E689" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F689" s="24"/>
     </row>
@@ -13717,10 +13721,10 @@
         <v>80</v>
       </c>
       <c r="D691" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E691" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F691" s="24"/>
     </row>
@@ -13788,7 +13792,7 @@
       </c>
       <c r="D696" s="17"/>
       <c r="E696" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F696" s="24"/>
     </row>
@@ -14050,10 +14054,10 @@
         <v>83</v>
       </c>
       <c r="D716" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E716" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="717" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14070,7 +14074,7 @@
         <v>16</v>
       </c>
       <c r="E717" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F717" s="24"/>
     </row>
@@ -14088,7 +14092,7 @@
         <v>27</v>
       </c>
       <c r="E718" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F718" s="24"/>
     </row>
@@ -14301,7 +14305,7 @@
         <v>27</v>
       </c>
       <c r="E734" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F734" s="46"/>
     </row>
@@ -14329,10 +14333,10 @@
         <v>86</v>
       </c>
       <c r="D736" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E736" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F736" s="24"/>
     </row>
@@ -14467,7 +14471,7 @@
         <v>16</v>
       </c>
       <c r="E746" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="747" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14559,10 +14563,10 @@
         <v>88</v>
       </c>
       <c r="D753" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E753" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F753" s="24"/>
     </row>
@@ -14571,7 +14575,7 @@
         <v>753</v>
       </c>
       <c r="B754" s="33" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C754" s="2">
         <v>88</v>
@@ -14616,10 +14620,10 @@
         <v>88</v>
       </c>
       <c r="D757" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E757" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F757" s="24"/>
     </row>
@@ -14648,7 +14652,7 @@
       </c>
       <c r="D759" s="17"/>
       <c r="E759" s="34" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="760" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14769,7 +14773,7 @@
         <v>16</v>
       </c>
       <c r="E768" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="769" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14836,7 +14840,7 @@
       </c>
       <c r="D773" s="17"/>
       <c r="E773" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F773" s="24"/>
     </row>
@@ -14893,7 +14897,7 @@
         <v>16</v>
       </c>
       <c r="E777" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F777" s="24"/>
     </row>
@@ -14947,10 +14951,10 @@
         <v>91</v>
       </c>
       <c r="D781" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E781" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F781" s="24"/>
     </row>
@@ -15017,10 +15021,10 @@
         <v>92</v>
       </c>
       <c r="D786" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E786" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F786" s="24"/>
     </row>
@@ -15051,7 +15055,7 @@
         <v>16</v>
       </c>
       <c r="E788" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F788" s="24"/>
     </row>
@@ -15157,7 +15161,7 @@
         <v>93</v>
       </c>
       <c r="D796" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E796" s="34"/>
     </row>
@@ -15725,7 +15729,7 @@
         <v>839</v>
       </c>
       <c r="B840" s="33" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C840" s="2">
         <v>98</v>
@@ -15773,7 +15777,7 @@
         <v>16</v>
       </c>
       <c r="E843" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="844" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -16047,10 +16051,10 @@
         <v>101</v>
       </c>
       <c r="D864" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E864" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F864" s="24"/>
     </row>
@@ -16117,7 +16121,7 @@
         <v>101</v>
       </c>
       <c r="D869" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E869" s="34"/>
     </row>
@@ -16135,7 +16139,7 @@
         <v>27</v>
       </c>
       <c r="E870" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F870" s="24"/>
     </row>
@@ -16229,7 +16233,7 @@
       </c>
       <c r="D877" s="17"/>
       <c r="E877" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F877" s="24"/>
     </row>
@@ -16244,10 +16248,10 @@
         <v>102</v>
       </c>
       <c r="D878" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E878" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F878" s="24"/>
     </row>
@@ -16314,10 +16318,10 @@
         <v>103</v>
       </c>
       <c r="D883" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E883" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F883" s="24"/>
     </row>
@@ -16374,7 +16378,7 @@
         <v>16</v>
       </c>
       <c r="E887" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F887" s="24"/>
     </row>
@@ -16519,10 +16523,10 @@
         <v>104</v>
       </c>
       <c r="D898" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E898" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F898" s="24"/>
     </row>
@@ -16602,10 +16606,10 @@
         <v>105</v>
       </c>
       <c r="D904" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E904" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F904" s="24"/>
     </row>
@@ -16816,7 +16820,7 @@
       </c>
       <c r="D920" s="17"/>
       <c r="E920" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F920" s="24"/>
     </row>
@@ -16987,10 +16991,10 @@
         <v>109</v>
       </c>
       <c r="D933" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E933" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F933" s="24"/>
     </row>
@@ -17057,10 +17061,10 @@
         <v>109</v>
       </c>
       <c r="D938" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E938" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F938" s="24"/>
     </row>
@@ -17091,7 +17095,7 @@
         <v>16</v>
       </c>
       <c r="E940" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F940" s="24"/>
     </row>
@@ -17172,7 +17176,7 @@
       </c>
       <c r="D946" s="17"/>
       <c r="E946" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F946" s="24"/>
     </row>
@@ -17291,10 +17295,10 @@
         <v>111</v>
       </c>
       <c r="D955" s="17" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="E955" s="34" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="956" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -17360,10 +17364,10 @@
         <v>112</v>
       </c>
       <c r="D960" s="17" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E960" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F960" s="24"/>
     </row>
@@ -17489,7 +17493,7 @@
         <v>969</v>
       </c>
       <c r="B970" s="33" t="s">
-        <v>959</v>
+        <v>1015</v>
       </c>
       <c r="C970" s="2">
         <v>113</v>
@@ -17502,7 +17506,7 @@
         <v>970</v>
       </c>
       <c r="B971" s="33" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C971" s="2">
         <v>113</v>
@@ -17515,7 +17519,7 @@
         <v>971</v>
       </c>
       <c r="B972" s="33" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C972" s="2">
         <v>113</v>
@@ -17528,7 +17532,7 @@
         <v>972</v>
       </c>
       <c r="B973" s="33" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C973" s="2">
         <v>113</v>
@@ -17541,7 +17545,7 @@
         <v>973</v>
       </c>
       <c r="B974" s="33" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C974" s="2">
         <v>113</v>
@@ -17554,7 +17558,7 @@
         <v>974</v>
       </c>
       <c r="B975" s="33" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C975" s="2">
         <v>113</v>
@@ -17567,7 +17571,7 @@
         <v>975</v>
       </c>
       <c r="B976" s="33" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C976" s="2">
         <v>113</v>
@@ -17580,7 +17584,7 @@
         <v>976</v>
       </c>
       <c r="B977" s="33" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C977" s="5">
         <v>114</v>
@@ -17593,7 +17597,7 @@
         <v>977</v>
       </c>
       <c r="B978" s="33" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C978" s="2">
         <v>114</v>
@@ -17606,7 +17610,7 @@
         <v>978</v>
       </c>
       <c r="B979" s="33" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C979" s="2">
         <v>114</v>
@@ -17619,7 +17623,7 @@
         <v>979</v>
       </c>
       <c r="B980" s="33" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C980" s="2">
         <v>114</v>
@@ -17632,7 +17636,7 @@
         <v>980</v>
       </c>
       <c r="B981" s="33" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C981" s="2">
         <v>114</v>
@@ -17645,7 +17649,7 @@
         <v>981</v>
       </c>
       <c r="B982" s="33" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C982" s="2">
         <v>114</v>
@@ -17658,7 +17662,7 @@
         <v>982</v>
       </c>
       <c r="B983" s="33" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C983" s="2">
         <v>114</v>
@@ -17671,7 +17675,7 @@
         <v>983</v>
       </c>
       <c r="B984" s="33" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C984" s="2">
         <v>114</v>
@@ -17684,7 +17688,7 @@
         <v>984</v>
       </c>
       <c r="B985" s="33" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C985" s="2">
         <v>114</v>
@@ -17697,7 +17701,7 @@
         <v>985</v>
       </c>
       <c r="B986" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C986" s="5">
         <v>115</v>
@@ -17710,7 +17714,7 @@
         <v>986</v>
       </c>
       <c r="B987" s="33" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C987" s="2">
         <v>115</v>
@@ -17723,7 +17727,7 @@
         <v>987</v>
       </c>
       <c r="B988" s="33" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C988" s="2">
         <v>115</v>
@@ -17736,7 +17740,7 @@
         <v>988</v>
       </c>
       <c r="B989" s="33" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C989" s="2">
         <v>115</v>
@@ -17749,7 +17753,7 @@
         <v>989</v>
       </c>
       <c r="B990" s="33" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C990" s="2">
         <v>115</v>
@@ -17762,7 +17766,7 @@
         <v>990</v>
       </c>
       <c r="B991" s="33" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C991" s="2">
         <v>115</v>
@@ -17775,7 +17779,7 @@
         <v>991</v>
       </c>
       <c r="B992" s="33" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C992" s="2">
         <v>115</v>
@@ -17788,7 +17792,7 @@
         <v>992</v>
       </c>
       <c r="B993" s="33" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C993" s="2">
         <v>115</v>
@@ -17803,7 +17807,7 @@
         <v>993</v>
       </c>
       <c r="B994" s="33" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C994" s="2">
         <v>115</v>
@@ -17816,16 +17820,16 @@
         <v>994</v>
       </c>
       <c r="B995" s="4" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C995" s="5">
         <v>116</v>
       </c>
       <c r="D995" s="17" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="E995" s="34" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F995" s="24"/>
     </row>
@@ -17834,7 +17838,7 @@
         <v>995</v>
       </c>
       <c r="B996" s="33" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C996" s="2">
         <v>116</v>
@@ -17847,7 +17851,7 @@
         <v>996</v>
       </c>
       <c r="B997" s="33" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C997" s="2">
         <v>116</v>
@@ -17860,7 +17864,7 @@
         <v>997</v>
       </c>
       <c r="B998" s="33" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C998" s="2">
         <v>116</v>
@@ -17873,7 +17877,7 @@
         <v>998</v>
       </c>
       <c r="B999" s="33" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C999" s="2">
         <v>116</v>
@@ -17888,7 +17892,7 @@
         <v>999</v>
       </c>
       <c r="B1000" s="33" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C1000" s="2">
         <v>116</v>
@@ -17901,7 +17905,7 @@
         <v>1000</v>
       </c>
       <c r="B1001" s="39" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C1001" s="40">
         <v>116</v>

</xml_diff>

<commit_message>
🎞 Boyz n the Hood
</commit_message>
<xml_diff>
--- a/CARTELERA.xlsx
+++ b/CARTELERA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54113\Desktop\CARTELERA 1000 PELICULAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBA32BA-3716-4B82-8623-44F5E8319E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C82C98-080D-4424-BE8A-E675394BDE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1016">
   <si>
     <t>PELÍCULA</t>
   </si>
@@ -3925,8 +3925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A515" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B529" sqref="B529"/>
+    <sheetView tabSelected="1" topLeftCell="A424" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E438" sqref="E438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3981,7 +3981,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="42">
         <f>COUNTIF($E$2:$E$1001,"VISTO")</f>
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="H5" s="13">
         <f>SUM(H2:H4)</f>
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4062,7 +4062,7 @@
       </c>
       <c r="H6" s="14">
         <f>1000-H5</f>
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4113,7 +4113,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="48" t="str">
         <f ca="1">INDEX(B2:B1001,RANDBETWEEN(1,COUNTA(B2:B1001)),1)</f>
-        <v>UP IN THE AIR</v>
+        <v>BELLA DE DÍA</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
@@ -10254,14 +10254,16 @@
       <c r="A437" s="31">
         <v>436</v>
       </c>
-      <c r="B437" s="33" t="s">
+      <c r="B437" s="35" t="s">
         <v>430</v>
       </c>
       <c r="C437" s="2">
         <v>52</v>
       </c>
       <c r="D437" s="17"/>
-      <c r="E437" s="34"/>
+      <c r="E437" s="34" t="s">
+        <v>1008</v>
+      </c>
     </row>
     <row r="438" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A438" s="31">

</xml_diff>

<commit_message>
🎞 EL SECRETO DE SUS OJOS
</commit_message>
<xml_diff>
--- a/CARTELERA.xlsx
+++ b/CARTELERA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\54113\Desktop\CARTELERA 1000 PELICULAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C82C98-080D-4424-BE8A-E675394BDE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA864FD-8931-4CD2-B4EA-6DFADA50D93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="1016">
   <si>
     <t>PELÍCULA</t>
   </si>
@@ -3925,8 +3927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E438" sqref="E438"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G250" sqref="G250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3981,7 +3983,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="42">
         <f>COUNTIF($E$2:$E$1001,"VISTO")</f>
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4039,7 +4041,7 @@
       </c>
       <c r="H5" s="13">
         <f>SUM(H2:H4)</f>
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4062,7 +4064,7 @@
       </c>
       <c r="H6" s="14">
         <f>1000-H5</f>
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4113,7 +4115,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="48" t="str">
         <f ca="1">INDEX(B2:B1001,RANDBETWEEN(1,COUNTA(B2:B1001)),1)</f>
-        <v>BELLA DE DÍA</v>
+        <v>LA PARADA DE LOS MONSTRUOS</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
@@ -7625,14 +7627,16 @@
       <c r="A253" s="31">
         <v>252</v>
       </c>
-      <c r="B253" s="33" t="s">
+      <c r="B253" s="35" t="s">
         <v>250</v>
       </c>
       <c r="C253" s="5">
         <v>31</v>
       </c>
       <c r="D253" s="17"/>
-      <c r="E253" s="34"/>
+      <c r="E253" s="34" t="s">
+        <v>1008</v>
+      </c>
     </row>
     <row r="254" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="31">

</xml_diff>

<commit_message>
🎞 THIS IS ENGLAND
</commit_message>
<xml_diff>
--- a/CARTELERA.xlsx
+++ b/CARTELERA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\OneDrive\Escritorio\CARTELERA 1000 PELICULAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A38757D-D504-428A-B2F1-8CFD80AAE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD97C0F-1152-4219-9ED3-2F5E594B98D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="1016">
   <si>
     <t>PELÍCULA</t>
   </si>
@@ -3927,8 +3927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B409" sqref="B409"/>
+    <sheetView tabSelected="1" topLeftCell="A440" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E456" sqref="E456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3983,7 +3983,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="42">
         <f>COUNTIF($E$2:$E$1001,"VISTO")</f>
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H5" s="13">
         <f>SUM(H2:H4)</f>
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4064,7 +4064,7 @@
       </c>
       <c r="H6" s="14">
         <f>1000-H5</f>
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4115,7 +4115,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="48" t="str">
         <f ca="1">INDEX(B2:B1001,RANDBETWEEN(1,COUNTA(B2:B1001)),1)</f>
-        <v>MASACRE</v>
+        <v>NADER Y SIMIN, UNA SEPARACIÓN</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
@@ -10500,14 +10500,16 @@
       <c r="A455" s="31">
         <v>454</v>
       </c>
-      <c r="B455" s="33" t="s">
+      <c r="B455" s="35" t="s">
         <v>447</v>
       </c>
       <c r="C455" s="2">
         <v>54</v>
       </c>
       <c r="D455" s="17"/>
-      <c r="E455" s="34"/>
+      <c r="E455" s="34" t="s">
+        <v>1007</v>
+      </c>
     </row>
     <row r="456" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A456" s="31">

</xml_diff>

<commit_message>
🎞️ THE DARK KNIGHT
</commit_message>
<xml_diff>
--- a/CARTELERA.xlsx
+++ b/CARTELERA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\OneDrive\Escritorio\CARTELERA 1000 PELICULAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483A7C0D-75F2-49E1-B6C7-A7E0A1396082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001F53CE-81CF-475F-9EA5-BF123607E0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="1016">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="1016">
   <si>
     <t>PELÍCULA</t>
   </si>
@@ -3927,8 +3927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A378" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B392" sqref="B392"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3983,7 +3983,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="42">
         <f>COUNTIF($E$2:$E$1001,"VISTO")</f>
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="H5" s="13">
         <f>SUM(H2:H4)</f>
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4064,7 +4064,7 @@
       </c>
       <c r="H6" s="14">
         <f>1000-H5</f>
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -4115,7 +4115,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="48" t="str">
         <f ca="1">INDEX(B2:B1001,RANDBETWEEN(1,COUNTA(B2:B1001)),1)</f>
-        <v>KRAMER CONTRA KRAMER</v>
+        <v>EL NUEVO ENTRENADOR</v>
       </c>
       <c r="H9" s="48"/>
       <c r="I9" s="48"/>
@@ -4581,14 +4581,16 @@
       <c r="A40" s="31">
         <v>39</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="2">
         <v>5</v>
       </c>
       <c r="D40" s="18"/>
-      <c r="E40" s="34"/>
+      <c r="E40" s="34" t="s">
+        <v>1007</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="31">

</xml_diff>